<commit_message>
Master fix relative path
</commit_message>
<xml_diff>
--- a/challengers_data_for_test/piggybank_test_binding.xlsx
+++ b/challengers_data_for_test/piggybank_test_binding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\thesis\testing\katalonproject\Challengers_C3_Katalon\challengers_data_for_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE7BABE-3314-4D54-A586-9BC0C614DE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED84D2D4-B21C-491E-B54B-CEDFD6288806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BAEF997D-F2D6-42B0-95AE-BAF202657A13}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BAEF997D-F2D6-42B0-95AE-BAF202657A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="G30" sqref="G30:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish create report + createe piggybank
</commit_message>
<xml_diff>
--- a/challengers_data_for_test/piggybank_test_binding.xlsx
+++ b/challengers_data_for_test/piggybank_test_binding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\thesis\testing\katalonproject\Challengers_C3_Katalon\challengers_data_for_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED84D2D4-B21C-491E-B54B-CEDFD6288806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D33266-4FC9-4D2A-AF82-AB6DF763E1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BAEF997D-F2D6-42B0-95AE-BAF202657A13}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="53">
   <si>
     <t>new_piggy_bank_notes</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>challengers_data_for_test\\piggybank\\Huytest64.txt</t>
+  </si>
+  <si>
+    <t>Buy Car Existed</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30:H30"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +675,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>

</xml_diff>